<commit_message>
Fix ADC issue and add one more taks to handler ADC
</commit_message>
<xml_diff>
--- a/DesignDocument/OBC软硬件接口(HSI)设计文档.xlsx
+++ b/DesignDocument/OBC软硬件接口(HSI)设计文档.xlsx
@@ -3,24 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6A3373-5AD2-441B-A908-E95ACB9D8488}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E552D68-4EDE-401D-901B-870BC89EFD04}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="SD Card" sheetId="2" r:id="rId2"/>
-    <sheet name="Clock" sheetId="3" r:id="rId3"/>
+    <sheet name="ADC" sheetId="4" r:id="rId2"/>
+    <sheet name="SD Card" sheetId="2" r:id="rId3"/>
+    <sheet name="Clock" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$D$1:$D$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$1:$F$65</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="274">
   <si>
     <t>Pin Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -426,10 +427,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ADC12_IN8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Red LED</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -931,6 +928,153 @@
   <si>
     <t>PPRE1</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMA Buffer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC_I_SET</t>
+  </si>
+  <si>
+    <t>ADC_C_SET</t>
+  </si>
+  <si>
+    <t>ADC_I_CHG</t>
+  </si>
+  <si>
+    <t>ADC_TEMP1</t>
+  </si>
+  <si>
+    <t>ADC_TEMP2</t>
+  </si>
+  <si>
+    <t>ADC_U_BAT</t>
+  </si>
+  <si>
+    <t>ADC_U_OUT</t>
+  </si>
+  <si>
+    <t>ADC_KEY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC_Channel_10</t>
+  </si>
+  <si>
+    <t>ADC_Channel_11</t>
+  </si>
+  <si>
+    <t>ADC_Channel_12</t>
+  </si>
+  <si>
+    <t>ADC_Channel_13</t>
+  </si>
+  <si>
+    <t>ADC_Channel_0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC_Channel_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC_Channel_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC_Channel_8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Signal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC Channel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Factor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Display</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC_SampleTime_55Cycles5</t>
+  </si>
+  <si>
+    <t>ADC_SampleTime_55Cycles5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Counter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test method： directly connect pin to GND，counter is nealy 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC12-Channel 14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC12-Channel 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC12-Channel 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC12-Channel 9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC_U_BAT_POS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC_U_BAT_NEG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC_Channel_14</t>
+  </si>
+  <si>
+    <t>ADC_Channel_15</t>
+  </si>
+  <si>
+    <t>ADC_Channel_9</t>
+  </si>
+  <si>
+    <t>ADC_V_CHG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC4</t>
+  </si>
+  <si>
+    <t>PC5</t>
   </si>
 </sst>
 </file>
@@ -982,7 +1126,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1001,8 +1145,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1025,11 +1175,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1044,6 +1205,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1637,7 +1802,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CEEACA"/>
+        <a:sysClr val="window" lastClr="CAEACE"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1953,8 +2118,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2107,7 +2272,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>28</v>
@@ -2115,6 +2280,7 @@
       <c r="F9" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -2127,7 +2293,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>29</v>
@@ -2135,6 +2301,7 @@
       <c r="F10" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -2147,7 +2314,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>30</v>
@@ -2155,6 +2322,7 @@
       <c r="F11" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -2167,7 +2335,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>31</v>
@@ -2175,6 +2343,7 @@
       <c r="F12" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -2216,7 +2385,7 @@
         <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>35</v>
@@ -2224,6 +2393,7 @@
       <c r="F15" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="G15" s="11"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2237,7 +2407,7 @@
         <v>27</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>39</v>
@@ -2245,6 +2415,7 @@
       <c r="F16" s="6" t="s">
         <v>45</v>
       </c>
+      <c r="G16" s="11"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2258,7 +2429,7 @@
         <v>27</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>47</v>
@@ -2266,6 +2437,7 @@
       <c r="F17" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="G17" s="11"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2322,16 +2494,16 @@
         <v>54</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2342,16 +2514,16 @@
         <v>55</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>129</v>
-      </c>
       <c r="F22" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>56</v>
@@ -2368,16 +2540,16 @@
         <v>60</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="E23" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>57</v>
@@ -2394,19 +2566,19 @@
         <v>61</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2419,8 +2591,11 @@
       <c r="E25" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2432,6 +2607,9 @@
       </c>
       <c r="E26" s="5" t="s">
         <v>105</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2445,16 +2623,17 @@
         <v>103</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2462,10 +2641,13 @@
         <v>65</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2479,10 +2661,10 @@
         <v>48</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2496,10 +2678,10 @@
         <v>48</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2513,10 +2695,10 @@
         <v>48</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2549,13 +2731,13 @@
         <v>71</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2566,13 +2748,13 @@
         <v>72</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2583,13 +2765,13 @@
         <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2603,13 +2785,13 @@
         <v>48</v>
       </c>
       <c r="D37" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="F37" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2623,13 +2805,13 @@
         <v>48</v>
       </c>
       <c r="D38" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="F38" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2640,10 +2822,10 @@
         <v>76</v>
       </c>
       <c r="C39" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>163</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="E39" s="6"/>
     </row>
@@ -2655,10 +2837,10 @@
         <v>77</v>
       </c>
       <c r="C40" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="E40" s="6"/>
     </row>
@@ -2670,10 +2852,10 @@
         <v>78</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E41" s="6"/>
     </row>
@@ -2685,10 +2867,10 @@
         <v>79</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2699,16 +2881,16 @@
         <v>80</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2719,16 +2901,16 @@
         <v>81</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2739,10 +2921,10 @@
         <v>82</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2753,10 +2935,10 @@
         <v>83</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2767,10 +2949,10 @@
         <v>84</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2781,10 +2963,10 @@
         <v>85</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2795,10 +2977,10 @@
         <v>86</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2809,7 +2991,7 @@
         <v>87</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2820,7 +3002,7 @@
         <v>88</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2831,10 +3013,10 @@
         <v>89</v>
       </c>
       <c r="C52" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2845,10 +3027,10 @@
         <v>90</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2859,10 +3041,10 @@
         <v>91</v>
       </c>
       <c r="C54" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2873,10 +3055,10 @@
         <v>92</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2887,7 +3069,7 @@
         <v>93</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2898,7 +3080,7 @@
         <v>94</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2909,7 +3091,7 @@
         <v>95</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2920,10 +3102,10 @@
         <v>96</v>
       </c>
       <c r="C59" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2934,10 +3116,10 @@
         <v>97</v>
       </c>
       <c r="C60" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2948,7 +3130,7 @@
         <v>98</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2959,7 +3141,7 @@
         <v>99</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2970,7 +3152,7 @@
         <v>100</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2981,10 +3163,10 @@
         <v>101</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2995,24 +3177,17 @@
         <v>102</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D65" xr:uid="{53DCED9C-1A61-4293-8B6C-5903FB453BD4}">
-    <filterColumn colId="0">
+  <autoFilter ref="A1:F65" xr:uid="{CF47E148-4D5C-4502-92EF-4AD199AF5190}">
+    <filterColumn colId="2">
       <filters>
-        <filter val="ADC_CSet_mV"/>
-        <filter val="ADC_ICharge_mA"/>
-        <filter val="ADC_ISet_mV"/>
-        <filter val="ADC_Temp1_mC"/>
-        <filter val="ADC_Temp2_mC"/>
-        <filter val="ADC_VBat_mV"/>
-        <filter val="ADC_Vkey_mV"/>
-        <filter val="ADC_VOut_mV"/>
+        <filter val="ADC"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3023,6 +3198,290 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091DB699-94B0-47D3-A036-E80D7C15C2B3}">
+  <dimension ref="A2:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>9</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="H12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>10</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="H13" t="s">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3038,7 +3497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:I45"/>
   <sheetViews>
@@ -3054,246 +3513,246 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B5">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B6">
         <f>B2*(B5+2)</f>
         <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B8">
         <f>B6</f>
         <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B10">
         <v>72</v>
       </c>
       <c r="C10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B12">
         <f>B10/2</f>
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B16">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B20">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B23">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B24">
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B27">
         <v>4</v>
@@ -3301,7 +3760,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -3309,18 +3768,18 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B33">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B34">
         <f>B35/(B18+1)</f>
@@ -3329,7 +3788,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B35">
         <f>B33/(B23+1)*(B24+2)</f>
@@ -3338,7 +3797,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B36">
         <f>B34*(B20+2)</f>
@@ -3347,7 +3806,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B37">
         <f>B36/(B27-2)</f>
@@ -3356,7 +3815,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B38">
         <f>B36*(B22+2)</f>
@@ -3365,24 +3824,24 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F43" t="s">
+        <v>199</v>
+      </c>
+      <c r="G43" t="s">
         <v>200</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>201</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>202</v>
-      </c>
-      <c r="I43" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E44">
         <f>B12/(1+F44+1+G44+1)/(H44+1)</f>

</xml_diff>